<commit_message>
recalc pop dens for FR cities, interpolating bw 2012 and 2017 and using 2010 for Paris
</commit_message>
<xml_diff>
--- a/outputs/density_geounits/summary_stats_Dijon.xlsx
+++ b/outputs/density_geounits/summary_stats_Dijon.xlsx
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>253637</v>
+        <v>252208</v>
       </c>
     </row>
     <row r="4">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1052.135608923543</v>
+        <v>1046.207838980074</v>
       </c>
     </row>
   </sheetData>

</xml_diff>